<commit_message>
generate primary signal of match table
</commit_message>
<xml_diff>
--- a/rv32_decode.xlsx
+++ b/rv32_decode.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\sheet_logic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FDA3FA-41C5-4BC0-BA40-BD9F40DD38B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3224D6-650D-406C-9F5B-48A040E172A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -479,7 +479,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>#flag(inst)</t>
+    <t>#primary(inst)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -622,12 +622,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -635,6 +629,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -992,15 +992,15 @@
       <c r="B6" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
@@ -1050,7 +1050,7 @@
       <c r="H8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="11" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1067,7 +1067,7 @@
       <c r="H9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="9"/>
+      <c r="I9" s="11"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
@@ -1132,7 +1132,7 @@
       <c r="H12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="I12" s="11" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1149,7 +1149,7 @@
       <c r="H13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I13" s="9"/>
+      <c r="I13" s="11"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="7"/>
@@ -1164,7 +1164,7 @@
       <c r="H14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I14" s="9"/>
+      <c r="I14" s="11"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="7"/>
@@ -1179,7 +1179,7 @@
       <c r="H15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I15" s="9"/>
+      <c r="I15" s="11"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="7"/>
@@ -1194,7 +1194,7 @@
       <c r="H16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I16" s="9"/>
+      <c r="I16" s="11"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="7"/>
@@ -1209,7 +1209,7 @@
       <c r="H17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I17" s="9"/>
+      <c r="I17" s="11"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
@@ -1230,7 +1230,7 @@
       <c r="H18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I18" s="9" t="s">
+      <c r="I18" s="11" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1247,7 +1247,7 @@
       <c r="H19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I19" s="9"/>
+      <c r="I19" s="11"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="7"/>
@@ -1262,7 +1262,7 @@
       <c r="H20" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I20" s="9"/>
+      <c r="I20" s="11"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="7"/>
@@ -1277,7 +1277,7 @@
       <c r="H21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I21" s="9"/>
+      <c r="I21" s="11"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="7"/>
@@ -1292,7 +1292,7 @@
       <c r="H22" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I22" s="9"/>
+      <c r="I22" s="11"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
@@ -1315,7 +1315,7 @@
       <c r="H23" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I23" s="9" t="s">
+      <c r="I23" s="11" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1332,7 +1332,7 @@
       <c r="H24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I24" s="9"/>
+      <c r="I24" s="11"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="7"/>
@@ -1347,7 +1347,7 @@
       <c r="H25" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I25" s="9"/>
+      <c r="I25" s="11"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
@@ -1368,7 +1368,7 @@
       <c r="H26" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I26" s="9" t="s">
+      <c r="I26" s="11" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1385,7 +1385,7 @@
       <c r="H27" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I27" s="9"/>
+      <c r="I27" s="11"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="7"/>
@@ -1400,7 +1400,7 @@
       <c r="H28" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I28" s="9"/>
+      <c r="I28" s="11"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="7"/>
@@ -1415,7 +1415,7 @@
       <c r="H29" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I29" s="9"/>
+      <c r="I29" s="11"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="7"/>
@@ -1430,7 +1430,7 @@
       <c r="H30" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I30" s="9"/>
+      <c r="I30" s="11"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="7"/>
@@ -1445,7 +1445,7 @@
       <c r="H31" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I31" s="9"/>
+      <c r="I31" s="11"/>
     </row>
     <row r="32" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
@@ -1464,7 +1464,7 @@
       <c r="H32" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I32" s="9"/>
+      <c r="I32" s="11"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="7"/>
@@ -1479,7 +1479,7 @@
       <c r="H33" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I33" s="9"/>
+      <c r="I33" s="11"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
@@ -1494,7 +1494,7 @@
       <c r="H34" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I34" s="9"/>
+      <c r="I34" s="11"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
@@ -1515,7 +1515,7 @@
       <c r="H35" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I35" s="9" t="s">
+      <c r="I35" s="11" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1532,7 +1532,7 @@
       <c r="H36" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I36" s="9"/>
+      <c r="I36" s="11"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
@@ -1549,7 +1549,7 @@
       <c r="H37" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I37" s="9"/>
+      <c r="I37" s="11"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="7"/>
@@ -1564,7 +1564,7 @@
       <c r="H38" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I38" s="9"/>
+      <c r="I38" s="11"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="7"/>
@@ -1579,7 +1579,7 @@
       <c r="H39" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I39" s="9"/>
+      <c r="I39" s="11"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="7"/>
@@ -1594,7 +1594,7 @@
       <c r="H40" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I40" s="9"/>
+      <c r="I40" s="11"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="7"/>
@@ -1609,7 +1609,7 @@
       <c r="H41" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I41" s="9"/>
+      <c r="I41" s="11"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
@@ -1624,7 +1624,7 @@
       <c r="H42" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I42" s="9"/>
+      <c r="I42" s="11"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="7" t="s">
@@ -1641,7 +1641,7 @@
       <c r="H43" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I43" s="9"/>
+      <c r="I43" s="11"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="7"/>
@@ -1656,7 +1656,7 @@
       <c r="H44" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="I44" s="9"/>
+      <c r="I44" s="11"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
@@ -1677,7 +1677,7 @@
       <c r="H45" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I45" s="9" t="s">
+      <c r="I45" s="11" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1694,7 +1694,7 @@
       <c r="H46" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I46" s="9"/>
+      <c r="I46" s="11"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
@@ -1715,7 +1715,7 @@
       <c r="H47" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I47" s="9"/>
+      <c r="I47" s="11"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="7" t="s">
@@ -1730,7 +1730,7 @@
       <c r="H48" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="I48" s="9"/>
+      <c r="I48" s="11"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="7" t="s">
@@ -1751,7 +1751,7 @@
       <c r="H49" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="I49" s="9"/>
+      <c r="I49" s="11"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="7"/>
@@ -1766,7 +1766,7 @@
       <c r="H50" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="I50" s="9"/>
+      <c r="I50" s="11"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="7"/>
@@ -1781,7 +1781,7 @@
       <c r="H51" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="I51" s="9"/>
+      <c r="I51" s="11"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="7"/>
@@ -1798,7 +1798,7 @@
       <c r="H52" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="I52" s="9"/>
+      <c r="I52" s="11"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="7"/>
@@ -1813,7 +1813,7 @@
       <c r="H53" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="I53" s="9"/>
+      <c r="I53" s="11"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="7"/>
@@ -1828,23 +1828,57 @@
       <c r="H54" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="I54" s="9"/>
+      <c r="I54" s="11"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A55" s="10" t="s">
+      <c r="A55" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="11"/>
-      <c r="F55" s="11"/>
-      <c r="G55" s="11"/>
-      <c r="H55" s="11"/>
-      <c r="I55" s="12"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9"/>
+      <c r="I55" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="F18:F22"/>
+    <mergeCell ref="E18:E22"/>
+    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="E12:E17"/>
+    <mergeCell ref="I12:I17"/>
+    <mergeCell ref="F12:F17"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="A8:D9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A18:B22"/>
+    <mergeCell ref="I26:I34"/>
+    <mergeCell ref="I35:I44"/>
+    <mergeCell ref="I45:I54"/>
+    <mergeCell ref="F26:F34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="G8:G54"/>
+    <mergeCell ref="E49:E54"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="I23:I25"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="I18:I22"/>
+    <mergeCell ref="A26:B31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="F35:F44"/>
+    <mergeCell ref="E26:E44"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="D41:D42"/>
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A48:B48"/>
@@ -1861,40 +1895,6 @@
     <mergeCell ref="E45:E48"/>
     <mergeCell ref="F45:F46"/>
     <mergeCell ref="F47:F54"/>
-    <mergeCell ref="A26:B31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="F35:F44"/>
-    <mergeCell ref="E26:E44"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="I26:I34"/>
-    <mergeCell ref="I35:I44"/>
-    <mergeCell ref="I45:I54"/>
-    <mergeCell ref="F26:F34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="G8:G54"/>
-    <mergeCell ref="E49:E54"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="I23:I25"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="I18:I22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="F18:F22"/>
-    <mergeCell ref="E18:E22"/>
-    <mergeCell ref="B12:B17"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="E12:E17"/>
-    <mergeCell ref="I12:I17"/>
-    <mergeCell ref="F12:F17"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="A8:D9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A18:B22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>